<commit_message>
Kenny had a stubbed out method, but I added my own method that accepts a message sent from the catch block that called ErrorLog, and the exception that goes along with it.
Utilized this ErrorLogger method and put calls to it in the catch blocks in ExcelImporterExporter.cs.
</commit_message>
<xml_diff>
--- a/ALF_Scheduler/TestData.xlsx
+++ b/ALF_Scheduler/TestData.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenny\Documents\GitHub\ALF_Scheduler\ALF_Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandtly\source\repos\ALF_Scheduler\ALF_Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD154FE-FE9A-4AE2-BA59-F5242394E8AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27000" windowHeight="13356"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>Facility Name</t>
   </si>
@@ -146,11 +153,128 @@
   <si>
     <t>YES</t>
   </si>
+  <si>
+    <t>APPLEWOOD TEST HOME</t>
+  </si>
+  <si>
+    <t>STROBECK, BRAN</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>9/31/2019</t>
+  </si>
+  <si>
+    <t>Test note, note note note.</t>
+  </si>
+  <si>
+    <t>BRIGHTON COURT</t>
+  </si>
+  <si>
+    <t>JOHANSSON, COLTON</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Notes for testing, hoorah.</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CHENEY ASSISTED LIVING</t>
+  </si>
+  <si>
+    <t>WILLIAMS,MICKI</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Cheney</t>
+  </si>
+  <si>
+    <t>Steiner</t>
+  </si>
+  <si>
+    <t>Capaul</t>
+  </si>
+  <si>
+    <t>Peters</t>
+  </si>
+  <si>
+    <t>(Testing enforcement notes)</t>
+  </si>
+  <si>
+    <t>CHERRYWOOD PLACE</t>
+  </si>
+  <si>
+    <t>DOE,JANE</t>
+  </si>
+  <si>
+    <t>Elon</t>
+  </si>
+  <si>
+    <t>No Enforcement/notes</t>
+  </si>
+  <si>
+    <t>EVERGREEN RESIDENTIAL CARE</t>
+  </si>
+  <si>
+    <t>SESSIONS, ADAM</t>
+  </si>
+  <si>
+    <t>Veradale</t>
+  </si>
+  <si>
+    <t>Leffen</t>
+  </si>
+  <si>
+    <t>Test test test test test</t>
+  </si>
+  <si>
+    <t>FAIRFIELD CARE</t>
+  </si>
+  <si>
+    <t>FUCHS, HELDA</t>
+  </si>
+  <si>
+    <t>Fairfield</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Armada</t>
+  </si>
+  <si>
+    <t>Testing Testing 1,2,3</t>
+  </si>
+  <si>
+    <t>MORAN VISTA ASSISTED LIVING</t>
+  </si>
+  <si>
+    <t>STEIGHNER, ANDREW</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>***TESTING***</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -811,38 +935,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="21" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="21"/>
-    <col min="7" max="7" width="10.109375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="21" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" style="21"/>
+    <col min="7" max="7" width="11.28515625" style="21" customWidth="1"/>
     <col min="8" max="8" width="12" style="21" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="21" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="21"/>
-    <col min="11" max="11" width="9.88671875" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="21" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" style="21" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="21"/>
-    <col min="15" max="15" width="12.6640625" style="21" customWidth="1"/>
-    <col min="16" max="16" width="25.5546875" style="21" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="21"/>
-    <col min="18" max="19" width="10.5546875" style="21" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" style="21" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="21"/>
+    <col min="9" max="9" width="11.140625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="21"/>
+    <col min="11" max="11" width="9.85546875" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="21" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="21"/>
+    <col min="15" max="15" width="12.7109375" style="21" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" style="21" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="21"/>
+    <col min="18" max="19" width="10.5703125" style="21" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="21" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +1034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>22</v>
       </c>
@@ -956,11 +1080,14 @@
       <c r="O2" s="22" t="s">
         <v>27</v>
       </c>
+      <c r="S2" s="22">
+        <v>20</v>
+      </c>
       <c r="U2" s="27">
         <v>43547</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
@@ -986,22 +1113,22 @@
         <v>43371</v>
       </c>
       <c r="I3" s="29">
-        <f>(H3 - G3) / 30.4</f>
+        <f t="shared" ref="I3:I10" si="0">(H3 - G3) / 30.4</f>
         <v>25.42763157894737</v>
       </c>
       <c r="J3" s="22">
-        <f>(H3 - G3)</f>
+        <f t="shared" ref="J3:J10" si="1">(H3 - G3)</f>
         <v>773</v>
       </c>
       <c r="K3" s="23">
         <v>43586</v>
       </c>
       <c r="L3" s="23">
-        <f>H3+517</f>
+        <f t="shared" ref="L3:L10" si="2">H3+517</f>
         <v>43888</v>
       </c>
       <c r="M3" s="23">
-        <f>H3+18*30.4</f>
+        <f t="shared" ref="M3:M10" si="3">H3+18*30.4</f>
         <v>43918.2</v>
       </c>
       <c r="N3" s="31" t="s">
@@ -1019,7 +1146,9 @@
       <c r="R3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="33">
+        <v>50</v>
+      </c>
       <c r="T3" s="32" t="s">
         <v>35</v>
       </c>
@@ -1027,40 +1156,516 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="22">
+        <v>321994</v>
+      </c>
+      <c r="E4" s="22">
+        <v>99203</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="23">
+        <v>42956</v>
+      </c>
+      <c r="H4" s="23">
+        <v>43355</v>
+      </c>
+      <c r="I4" s="29">
+        <f t="shared" si="0"/>
+        <v>13.125</v>
+      </c>
+      <c r="J4" s="22">
+        <f t="shared" si="1"/>
+        <v>399</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="23">
+        <f t="shared" si="2"/>
+        <v>43872</v>
+      </c>
+      <c r="M4" s="23">
+        <f t="shared" si="3"/>
+        <v>43902.2</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="22">
+        <v>75</v>
+      </c>
+      <c r="T4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="22">
+        <v>123789</v>
+      </c>
+      <c r="E5" s="22">
+        <v>99216</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="23">
+        <v>43066</v>
+      </c>
+      <c r="H5" s="23">
+        <v>43109</v>
+      </c>
+      <c r="I5" s="29">
+        <f t="shared" si="0"/>
+        <v>1.4144736842105263</v>
+      </c>
+      <c r="J5" s="22">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="K5" s="23">
+        <v>43468</v>
+      </c>
+      <c r="L5" s="23">
+        <f t="shared" si="2"/>
+        <v>43626</v>
+      </c>
+      <c r="M5" s="23">
+        <f t="shared" si="3"/>
+        <v>43656.2</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="22">
+        <v>8</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="23">
+        <v>43468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="22">
+        <v>13267</v>
+      </c>
+      <c r="E6" s="22">
+        <v>99004</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="23">
+        <v>43339</v>
+      </c>
+      <c r="H6" s="23">
+        <v>43409</v>
+      </c>
+      <c r="I6" s="29">
+        <f t="shared" si="0"/>
+        <v>2.3026315789473686</v>
+      </c>
+      <c r="J6" s="22">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="K6" s="23">
+        <v>43801</v>
+      </c>
+      <c r="L6" s="23">
+        <f t="shared" si="2"/>
+        <v>43926</v>
+      </c>
+      <c r="M6" s="23">
+        <f t="shared" si="3"/>
+        <v>43956.2</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="22">
+        <v>25</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="23">
+        <v>43801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="22">
+        <v>2434</v>
+      </c>
+      <c r="E7" s="22">
+        <v>99208</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="23">
+        <v>43011</v>
+      </c>
+      <c r="H7" s="23">
+        <v>43180</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" si="0"/>
+        <v>5.5592105263157894</v>
+      </c>
+      <c r="J7" s="22">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+      <c r="K7" s="23">
+        <v>43575</v>
+      </c>
+      <c r="L7" s="23">
+        <f t="shared" si="2"/>
+        <v>43697</v>
+      </c>
+      <c r="M7" s="23">
+        <f t="shared" si="3"/>
+        <v>43727.199999999997</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="22">
+        <v>88</v>
+      </c>
+      <c r="T7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="23">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="22">
+        <v>2138</v>
+      </c>
+      <c r="E8" s="22">
+        <v>99037</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="23">
+        <v>43166</v>
+      </c>
+      <c r="H8" s="23">
+        <v>43199</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="0"/>
+        <v>1.0855263157894737</v>
+      </c>
+      <c r="J8" s="22">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K8" s="23">
+        <v>43564</v>
+      </c>
+      <c r="L8" s="23">
+        <f t="shared" si="2"/>
+        <v>43716</v>
+      </c>
+      <c r="M8" s="23">
+        <f t="shared" si="3"/>
+        <v>43746.2</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="22">
+        <v>99</v>
+      </c>
+      <c r="T8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8" s="23">
+        <v>43564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="22">
+        <v>2128</v>
+      </c>
+      <c r="E9" s="22">
+        <v>99012</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="23">
+        <v>43370</v>
+      </c>
+      <c r="H9" s="23">
+        <v>43447</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5328947368421053</v>
+      </c>
+      <c r="J9" s="22">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="K9" s="23">
+        <v>43629</v>
+      </c>
+      <c r="L9" s="23">
+        <f t="shared" si="2"/>
+        <v>43964</v>
+      </c>
+      <c r="M9" s="23">
+        <f t="shared" si="3"/>
+        <v>43994.2</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="22">
+        <v>111</v>
+      </c>
+      <c r="T9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="23">
+        <v>43629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1987</v>
+      </c>
+      <c r="E10" s="22">
+        <v>99223</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="23">
+        <v>42209</v>
+      </c>
+      <c r="H10" s="23">
+        <v>42594</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="0"/>
+        <v>12.664473684210527</v>
+      </c>
+      <c r="J10" s="22">
+        <f t="shared" si="1"/>
+        <v>385</v>
+      </c>
+      <c r="K10" s="23">
+        <v>43507</v>
+      </c>
+      <c r="L10" s="23">
+        <f t="shared" si="2"/>
+        <v>43111</v>
+      </c>
+      <c r="M10" s="23">
+        <f t="shared" si="3"/>
+        <v>43141.2</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="22">
+        <v>76</v>
+      </c>
+      <c r="T10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U10" s="23">
+        <v>43507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Had to change the test excel to not be read-only
</commit_message>
<xml_diff>
--- a/ALF_Scheduler/TestData.xlsx
+++ b/ALF_Scheduler/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandtly\source\repos\ALF_Scheduler\ALF_Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD154FE-FE9A-4AE2-BA59-F5242394E8AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211659DF-AEAC-46FC-9586-79E31A110ED2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,25 +275,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,147 +292,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0066FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC6600"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3399"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9933FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99CC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -455,159 +308,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,736 +642,704 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="21" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" style="21"/>
-    <col min="7" max="7" width="11.28515625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="12" style="21" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="21" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="21"/>
-    <col min="11" max="11" width="9.85546875" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="21" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="21" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="21"/>
-    <col min="15" max="15" width="12.7109375" style="21" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="21"/>
-    <col min="18" max="19" width="10.5703125" style="21" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="21" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="18" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2">
         <v>725103</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2">
         <v>98001</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2">
         <v>42230</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2">
         <v>43154</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2">
         <v>18.36</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2">
         <v>558</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2">
         <v>43547</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2">
         <v>43671</v>
       </c>
-      <c r="M2" s="26">
+      <c r="M2">
         <v>43702</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="22">
+      <c r="S2">
         <v>20</v>
       </c>
-      <c r="U2" s="27">
+      <c r="U2">
         <v>43547</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3">
         <v>843121</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3">
         <v>99208</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3">
         <v>42598</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3">
         <v>43371</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3">
         <f t="shared" ref="I3:I10" si="0">(H3 - G3) / 30.4</f>
         <v>25.42763157894737</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3">
         <f t="shared" ref="J3:J10" si="1">(H3 - G3)</f>
         <v>773</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3">
         <v>43586</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3">
         <f t="shared" ref="L3:L10" si="2">H3+517</f>
         <v>43888</v>
       </c>
-      <c r="M3" s="23">
+      <c r="M3">
         <f t="shared" ref="M3:M10" si="3">H3+18*30.4</f>
         <v>43918.2</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="33">
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3">
         <v>50</v>
       </c>
-      <c r="T3" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="27">
+      <c r="T3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3">
         <v>43586</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4">
         <v>321994</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4">
         <v>99203</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4">
         <v>42956</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4">
         <v>43355</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>13.125</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4">
         <f t="shared" si="1"/>
         <v>399</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4">
         <f t="shared" si="2"/>
         <v>43872</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4">
         <f t="shared" si="3"/>
         <v>43902.2</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="22">
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4">
         <v>75</v>
       </c>
-      <c r="T4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="22" t="s">
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5">
         <v>123789</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5">
         <v>99216</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5">
         <v>43066</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5">
         <v>43109</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>1.4144736842105263</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5">
         <v>43468</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5">
         <f t="shared" si="2"/>
         <v>43626</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5">
         <f t="shared" si="3"/>
         <v>43656.2</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="22">
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5">
         <v>8</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" t="s">
         <v>46</v>
       </c>
-      <c r="U5" s="23">
+      <c r="U5">
         <v>43468</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6">
         <v>13267</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6">
         <v>99004</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6">
         <v>43339</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6">
         <v>43409</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>2.3026315789473686</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6">
         <v>43801</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6">
         <f t="shared" si="2"/>
         <v>43926</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6">
         <f t="shared" si="3"/>
         <v>43956.2</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="22" t="s">
+      <c r="O6" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" s="22">
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6">
         <v>25</v>
       </c>
-      <c r="T6" s="22" t="s">
+      <c r="T6" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="23">
+      <c r="U6">
         <v>43801</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7">
         <v>2434</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7">
         <v>99208</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7">
         <v>43011</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7">
         <v>43180</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>5.5592105263157894</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7">
         <f t="shared" si="1"/>
         <v>169</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7">
         <v>43575</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7">
         <f t="shared" si="2"/>
         <v>43697</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7">
         <f t="shared" si="3"/>
         <v>43727.199999999997</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="N7" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="O7" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="22">
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7">
         <v>88</v>
       </c>
-      <c r="T7" s="22" t="s">
+      <c r="T7" t="s">
         <v>46</v>
       </c>
-      <c r="U7" s="23">
+      <c r="U7">
         <v>43575</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8">
         <v>2138</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8">
         <v>99037</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8">
         <v>43166</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8">
         <v>43199</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>1.0855263157894737</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8">
         <v>43564</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8">
         <f t="shared" si="2"/>
         <v>43716</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8">
         <f t="shared" si="3"/>
         <v>43746.2</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" t="s">
         <v>46</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" t="s">
         <v>63</v>
       </c>
-      <c r="Q8" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" s="22">
+      <c r="Q8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8">
         <v>99</v>
       </c>
-      <c r="T8" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="U8" s="23">
+      <c r="T8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8">
         <v>43564</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9">
         <v>2128</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9">
         <v>99012</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9">
         <v>43370</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9">
         <v>43447</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>2.5328947368421053</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9">
         <v>43629</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9">
         <f t="shared" si="2"/>
         <v>43964</v>
       </c>
-      <c r="M9" s="23">
+      <c r="M9">
         <f t="shared" si="3"/>
         <v>43994.2</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" t="s">
         <v>68</v>
       </c>
-      <c r="O9" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="22" t="s">
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" t="s">
         <v>69</v>
       </c>
-      <c r="Q9" s="22" t="s">
+      <c r="Q9" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S9" s="22">
+      <c r="R9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9">
         <v>111</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" t="s">
         <v>46</v>
       </c>
-      <c r="U9" s="23">
+      <c r="U9">
         <v>43629</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10">
         <v>1987</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10">
         <v>99223</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10">
         <v>42209</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10">
         <v>42594</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>12.664473684210527</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10">
         <f t="shared" si="1"/>
         <v>385</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10">
         <v>43507</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10">
         <f t="shared" si="2"/>
         <v>43111</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10">
         <f t="shared" si="3"/>
         <v>43141.2</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="N10" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="22" t="s">
+      <c r="O10" t="s">
         <v>46</v>
       </c>
-      <c r="P10" s="22" t="s">
+      <c r="P10" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="22" t="s">
+      <c r="Q10" t="s">
         <v>46</v>
       </c>
-      <c r="R10" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" s="22">
+      <c r="R10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10">
         <v>76</v>
       </c>
-      <c r="T10" s="22" t="s">
+      <c r="T10" t="s">
         <v>46</v>
       </c>
-      <c r="U10" s="23">
+      <c r="U10">
         <v>43507</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>